<commit_message>
added file OECD-happiness... with Cannabis, Cocaine, and Tertiary Education stats of OECD countries. Will add Antidepressant use later tonight
</commit_message>
<xml_diff>
--- a/Stephanie/happiness-correlations-steph.xlsx
+++ b/Stephanie/happiness-correlations-steph.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniemark/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniemark/Documents/SP18/INFO 3300/3300-p1/Stephanie/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="1240" windowWidth="22160" windowHeight="16540" activeTab="2" xr2:uid="{05585DEE-E31A-F647-82F2-51A3607B14A8}"/>
+    <workbookView xWindow="1760" yWindow="460" windowWidth="22160" windowHeight="16540" activeTab="2" xr2:uid="{05585DEE-E31A-F647-82F2-51A3607B14A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Happiness + Education Level" sheetId="1" r:id="rId1"/>
     <sheet name="Happiness + Patriotism" sheetId="2" r:id="rId2"/>
     <sheet name="Happiness + Drug Use" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -853,542 +853,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DEDAD6F3-723B-8546-B879-147C4B4C9D95}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{8561D531-EB24-2945-8D95-72609FC05652}"/>
   </cellStyles>
-  <dxfs count="119">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1743,7 +1208,7 @@
         <v>7.5370001792907715</v>
       </c>
       <c r="C2">
-        <f>INDEX(I:I, MATCH(A2, H:H, 0))</f>
+        <f t="shared" ref="C2:C27" si="0">INDEX(I:I, MATCH(A2, H:H, 0))</f>
         <v>42</v>
       </c>
       <c r="H2" t="s">
@@ -1761,7 +1226,7 @@
         <v>7.5219998359680176</v>
       </c>
       <c r="C3">
-        <f>INDEX(I:I, MATCH(A3, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="H3" t="s">
@@ -1779,7 +1244,7 @@
         <v>7.504000186920166</v>
       </c>
       <c r="C4">
-        <f>INDEX(I:I, MATCH(A4, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="H4" t="s">
@@ -1797,7 +1262,7 @@
         <v>7.4689998626708984</v>
       </c>
       <c r="C5">
-        <f>INDEX(I:I, MATCH(A5, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="H5" t="s">
@@ -1815,7 +1280,7 @@
         <v>7.3769998550415039</v>
       </c>
       <c r="C6">
-        <f>INDEX(I:I, MATCH(A6, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="H6" t="s">
@@ -1833,7 +1298,7 @@
         <v>7.3159999847412109</v>
       </c>
       <c r="C7">
-        <f>INDEX(I:I, MATCH(A7, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="H7" t="s">
@@ -1851,7 +1316,7 @@
         <v>7.314000129699707</v>
       </c>
       <c r="C8">
-        <f>INDEX(I:I, MATCH(A8, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="H8" t="s">
@@ -1869,7 +1334,7 @@
         <v>7.2839999198913574</v>
       </c>
       <c r="C9">
-        <f>INDEX(I:I, MATCH(A9, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="H9" t="s">
@@ -1887,7 +1352,7 @@
         <v>7.2129998207092285</v>
       </c>
       <c r="C10">
-        <f>INDEX(I:I, MATCH(A10, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="H10" t="s">
@@ -1905,7 +1370,7 @@
         <v>7.0789999961853027</v>
       </c>
       <c r="C11">
-        <f>INDEX(I:I, MATCH(A11, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="H11" t="s">
@@ -1923,7 +1388,7 @@
         <v>7.0060000419616699</v>
       </c>
       <c r="C12">
-        <f>INDEX(I:I, MATCH(A12, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="H12" t="s">
@@ -1941,7 +1406,7 @@
         <v>6.9770002365112305</v>
       </c>
       <c r="C13">
-        <f>INDEX(I:I, MATCH(A13, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="H13" t="s">
@@ -1959,7 +1424,7 @@
         <v>6.9510002136230469</v>
       </c>
       <c r="C14">
-        <f>INDEX(I:I, MATCH(A14, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="H14" t="s">
@@ -1977,7 +1442,7 @@
         <v>6.8909997940063477</v>
       </c>
       <c r="C15">
-        <f>INDEX(I:I, MATCH(A15, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="H15" t="s">
@@ -1995,7 +1460,7 @@
         <v>6.8629999160766602</v>
       </c>
       <c r="C16">
-        <f>INDEX(I:I, MATCH(A16, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="H16" t="s">
@@ -2013,7 +1478,7 @@
         <v>6.6519999504089355</v>
       </c>
       <c r="C17">
-        <f>INDEX(I:I, MATCH(A17, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="H17" t="s">
@@ -2031,7 +1496,7 @@
         <v>6.6350002288818359</v>
       </c>
       <c r="C18">
-        <f>INDEX(I:I, MATCH(A18, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="H18" t="s">
@@ -2049,7 +1514,7 @@
         <v>6.6090002059936523</v>
       </c>
       <c r="C19">
-        <f>INDEX(I:I, MATCH(A19, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="H19" t="s">
@@ -2067,7 +1532,7 @@
         <v>6.5780000686645508</v>
       </c>
       <c r="C20">
-        <f>INDEX(I:I, MATCH(A20, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="H20" t="s">
@@ -2085,7 +1550,7 @@
         <v>6.4419999122619629</v>
       </c>
       <c r="C21">
-        <f>INDEX(I:I, MATCH(A21, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="H21" t="s">
@@ -2103,7 +1568,7 @@
         <v>5.8499999046325684</v>
       </c>
       <c r="C22">
-        <f>INDEX(I:I, MATCH(A22, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="H22" t="s">
@@ -2121,7 +1586,7 @@
         <v>5.6110000610351562</v>
       </c>
       <c r="C23">
-        <f>INDEX(I:I, MATCH(A23, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="H23" t="s">
@@ -2139,7 +1604,7 @@
         <v>5.3239998817443848</v>
       </c>
       <c r="C24">
-        <f>INDEX(I:I, MATCH(A24, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="H24" t="s">
@@ -2157,7 +1622,7 @@
         <v>5.2729997634887695</v>
       </c>
       <c r="C25">
-        <f>INDEX(I:I, MATCH(A25, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H25" t="s">
@@ -2175,7 +1640,7 @@
         <v>5.2620000839233398</v>
       </c>
       <c r="C26">
-        <f>INDEX(I:I, MATCH(A26, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H26" t="s">
@@ -2193,7 +1658,7 @@
         <v>5.2270002365112305</v>
       </c>
       <c r="C27">
-        <f>INDEX(I:I, MATCH(A27, H:H, 0))</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="H27" t="s">
@@ -2745,7 +2210,7 @@
   <dimension ref="A1:Q299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2759,7 +2224,7 @@
     <col min="17" max="17" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="112" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="96" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2799,7 +2264,7 @@
         <v>7.5370001792907715</v>
       </c>
       <c r="C2">
-        <f>INDEX(L:L, MATCH(A2, K:K, 0))</f>
+        <f t="shared" ref="C2:C33" si="0">INDEX(L:L, MATCH(A2, K:K, 0))</f>
         <v>4.2</v>
       </c>
       <c r="E2">
@@ -2821,11 +2286,11 @@
         <v>7.5219998359680176</v>
       </c>
       <c r="C3">
-        <f>INDEX(L:L, MATCH(A3, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>6.9</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="0">INDEX(O:O, MATCH(A3, K:K, 0))</f>
+        <f t="shared" ref="E3:E66" si="1">INDEX(O:O, MATCH(A3, K:K, 0))</f>
         <v>1.7</v>
       </c>
       <c r="K3" t="s">
@@ -2843,11 +2308,11 @@
         <v>7.504000186920166</v>
       </c>
       <c r="C4">
-        <f>INDEX(L:L, MATCH(A4, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>18.3</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="K4" t="s">
@@ -2865,11 +2330,11 @@
         <v>7.4939999580383301</v>
       </c>
       <c r="C5">
-        <f>INDEX(L:L, MATCH(A5, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>6.7</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K5" t="s">
@@ -2887,11 +2352,11 @@
         <v>7.4689998626708984</v>
       </c>
       <c r="C6">
-        <f>INDEX(L:L, MATCH(A6, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="K6" t="s">
@@ -2909,11 +2374,11 @@
         <v>7.3769998550415039</v>
       </c>
       <c r="C7">
-        <f>INDEX(L:L, MATCH(A7, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="K7" t="s">
@@ -2937,11 +2402,11 @@
         <v>7.3159999847412109</v>
       </c>
       <c r="C8">
-        <f>INDEX(L:L, MATCH(A8, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>12.7</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K8" t="s">
@@ -2962,11 +2427,11 @@
         <v>7.314000129699707</v>
       </c>
       <c r="C9">
-        <f>INDEX(L:L, MATCH(A9, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K9" t="s">
@@ -2987,11 +2452,11 @@
         <v>7.2839999198913574</v>
       </c>
       <c r="C10">
-        <f>INDEX(L:L, MATCH(A10, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>2.88</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K10" t="s">
@@ -3012,11 +2477,11 @@
         <v>7.2839999198913574</v>
       </c>
       <c r="C11">
-        <f>INDEX(L:L, MATCH(A11, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>10.199999999999999</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K11" t="s">
@@ -3037,11 +2502,11 @@
         <v>7.2129998207092285</v>
       </c>
       <c r="C12">
-        <f>INDEX(L:L, MATCH(A12, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>8.8800000000000008</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K12" t="s">
@@ -3059,11 +2524,11 @@
         <v>7.0789999961853027</v>
       </c>
       <c r="C13">
-        <f>INDEX(L:L, MATCH(A13, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>2.76</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.69</v>
       </c>
       <c r="K13" t="s">
@@ -3081,11 +2546,11 @@
         <v>7.0060000419616699</v>
       </c>
       <c r="C14">
-        <f>INDEX(L:L, MATCH(A14, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="K14" t="s">
@@ -3103,11 +2568,11 @@
         <v>6.9770002365112305</v>
       </c>
       <c r="C15">
-        <f>INDEX(L:L, MATCH(A15, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
       <c r="K15" t="s">
@@ -3128,11 +2593,11 @@
         <v>6.9510002136230469</v>
       </c>
       <c r="C16">
-        <f>INDEX(L:L, MATCH(A16, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.04</v>
       </c>
       <c r="K16" t="s">
@@ -3153,11 +2618,11 @@
         <v>6.8909997940063477</v>
       </c>
       <c r="C17">
-        <f>INDEX(L:L, MATCH(A17, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K17" t="s">
@@ -3178,11 +2643,11 @@
         <v>6.8629999160766602</v>
       </c>
       <c r="C18">
-        <f>INDEX(L:L, MATCH(A18, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>5.2</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="K18" t="s">
@@ -3206,11 +2671,11 @@
         <v>6.6519999504089355</v>
       </c>
       <c r="C19">
-        <f>INDEX(L:L, MATCH(A19, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>11.83</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K19" t="s">
@@ -3228,11 +2693,11 @@
         <v>6.6479997634887695</v>
       </c>
       <c r="C20">
-        <f>INDEX(L:L, MATCH(A20, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>5.35</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="K20" t="s">
@@ -3253,11 +2718,11 @@
         <v>6.6090002059936523</v>
       </c>
       <c r="C21">
-        <f>INDEX(L:L, MATCH(A21, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>8.9</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.88</v>
       </c>
       <c r="K21" t="s">
@@ -3275,11 +2740,11 @@
         <v>6.5989999771118164</v>
       </c>
       <c r="C22">
-        <f>INDEX(L:L, MATCH(A22, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="K22" t="s">
@@ -3297,11 +2762,11 @@
         <v>6.5780000686645508</v>
       </c>
       <c r="C23">
-        <f>INDEX(L:L, MATCH(A23, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="K23" t="s">
@@ -3322,11 +2787,11 @@
         <v>6.5720000267028809</v>
       </c>
       <c r="C24">
-        <f>INDEX(L:L, MATCH(A24, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K24" t="s">
@@ -3344,11 +2809,11 @@
         <v>6.5269999504089355</v>
       </c>
       <c r="C25">
-        <f>INDEX(L:L, MATCH(A25, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.38</v>
       </c>
       <c r="K25" t="s">
@@ -3366,11 +2831,11 @@
         <v>6.4539999961853027</v>
       </c>
       <c r="C26">
-        <f>INDEX(L:L, MATCH(A26, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>9.3000000000000007</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K26" t="s">
@@ -3388,11 +2853,11 @@
         <v>6.4539999961853027</v>
       </c>
       <c r="C27">
-        <f>INDEX(L:L, MATCH(A27, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="K27" t="s">
@@ -3410,11 +2875,11 @@
         <v>6.4520001411437988</v>
       </c>
       <c r="C28">
-        <f>INDEX(L:L, MATCH(A28, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>3.55</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.73</v>
       </c>
       <c r="K28" t="s">
@@ -3432,11 +2897,11 @@
         <v>6.4419999122619629</v>
       </c>
       <c r="C29">
-        <f>INDEX(L:L, MATCH(A29, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>11.1</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="K29" t="s">
@@ -3454,11 +2919,11 @@
         <v>6.4239997863769531</v>
       </c>
       <c r="C30">
-        <f>INDEX(L:L, MATCH(A30, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
       <c r="K30" t="s">
@@ -3479,11 +2944,11 @@
         <v>6.4219999313354492</v>
       </c>
       <c r="C31">
-        <f>INDEX(L:L, MATCH(A31, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K31" t="s">
@@ -3504,11 +2969,11 @@
         <v>6.4029998779296875</v>
       </c>
       <c r="C32">
-        <f>INDEX(L:L, MATCH(A32, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>9.1999999999999993</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K32" t="s">
@@ -3529,11 +2994,11 @@
         <v>6.3569998741149902</v>
       </c>
       <c r="C33">
-        <f>INDEX(L:L, MATCH(A33, K:K, 0))</f>
+        <f t="shared" si="0"/>
         <v>3.27</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="K33" t="s">
@@ -3554,11 +3019,11 @@
         <v>6.3439998626708984</v>
       </c>
       <c r="C34">
-        <f>INDEX(L:L, MATCH(A34, K:K, 0))</f>
+        <f t="shared" ref="C34:C65" si="2">INDEX(L:L, MATCH(A34, K:K, 0))</f>
         <v>0.3</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
       <c r="K34" t="s">
@@ -3576,11 +3041,11 @@
         <v>6.1680002212524414</v>
       </c>
       <c r="C35">
-        <f>INDEX(L:L, MATCH(A35, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>4.03</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.31</v>
       </c>
       <c r="K35" t="s">
@@ -3601,11 +3066,11 @@
         <v>6.1050000190734863</v>
       </c>
       <c r="C36">
-        <f>INDEX(L:L, MATCH(A36, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K36" t="s">
@@ -3626,11 +3091,11 @@
         <v>6.0980000495910645</v>
       </c>
       <c r="C37">
-        <f>INDEX(L:L, MATCH(A37, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>3.63</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1</v>
       </c>
       <c r="K37" t="s">
@@ -3651,11 +3116,11 @@
         <v>6.0840001106262207</v>
       </c>
       <c r="C38">
-        <f>INDEX(L:L, MATCH(A38, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
       <c r="K38" t="s">
@@ -3676,11 +3141,11 @@
         <v>6.0710000991821289</v>
       </c>
       <c r="C39">
-        <f>INDEX(L:L, MATCH(A39, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>1.07</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1</v>
       </c>
       <c r="K39" t="s">
@@ -3701,11 +3166,11 @@
         <v>6.0079998970031738</v>
       </c>
       <c r="C40">
-        <f>INDEX(L:L, MATCH(A40, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>0.67</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="K40" t="s">
@@ -3726,11 +3191,11 @@
         <v>6.0029997825622559</v>
       </c>
       <c r="C41">
-        <f>INDEX(L:L, MATCH(A41, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>2.0299999999999998</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K41" t="s">
@@ -3751,11 +3216,11 @@
         <v>5.9730000495910645</v>
       </c>
       <c r="C42">
-        <f>INDEX(L:L, MATCH(A42, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
       <c r="K42" t="s">
@@ -3773,11 +3238,11 @@
         <v>5.9710001945495605</v>
       </c>
       <c r="C43">
-        <f>INDEX(L:L, MATCH(A43, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>4.2</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K43" t="s">
@@ -3795,11 +3260,11 @@
         <v>5.9640002250671387</v>
       </c>
       <c r="C44">
-        <f>INDEX(L:L, MATCH(A44, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>9.1999999999999993</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="K44" t="s">
@@ -3817,11 +3282,11 @@
         <v>5.9559998512268066</v>
       </c>
       <c r="C45">
-        <f>INDEX(L:L, MATCH(A45, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>8.4499999999999993</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.87</v>
       </c>
       <c r="K45" t="s">
@@ -3839,11 +3304,11 @@
         <v>5.9200000762939453</v>
       </c>
       <c r="C46">
-        <f>INDEX(L:L, MATCH(A46, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K46" t="s">
@@ -3861,11 +3326,11 @@
         <v>5.9019999504089355</v>
       </c>
       <c r="C47">
-        <f>INDEX(L:L, MATCH(A47, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="K47" t="s">
@@ -3883,11 +3348,11 @@
         <v>5.8720002174377441</v>
       </c>
       <c r="C48">
-        <f>INDEX(L:L, MATCH(A48, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>0.52</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K48" t="s">
@@ -3905,11 +3370,11 @@
         <v>5.8499999046325684</v>
       </c>
       <c r="C49">
-        <f>INDEX(L:L, MATCH(A49, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K49" t="s">
@@ -3927,11 +3392,11 @@
         <v>5.8249998092651367</v>
       </c>
       <c r="C50">
-        <f>INDEX(L:L, MATCH(A50, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
       <c r="K50" t="s">
@@ -3949,11 +3414,11 @@
         <v>5.8220000267028809</v>
       </c>
       <c r="C51">
-        <f>INDEX(L:L, MATCH(A51, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K51" t="s">
@@ -3971,11 +3436,11 @@
         <v>5.8189997673034668</v>
       </c>
       <c r="C52">
-        <f>INDEX(L:L, MATCH(A52, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>2.4</v>
       </c>
       <c r="E52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K52" t="s">
@@ -3993,11 +3458,11 @@
         <v>5.7579998970031738</v>
       </c>
       <c r="C53">
-        <f>INDEX(L:L, MATCH(A53, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K53" t="s">
@@ -4015,11 +3480,11 @@
         <v>5.7150001525878906</v>
       </c>
       <c r="C54">
-        <f>INDEX(L:L, MATCH(A54, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>1.03</v>
       </c>
       <c r="E54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K54" t="s">
@@ -4040,11 +3505,11 @@
         <v>5.629000186920166</v>
       </c>
       <c r="C55">
-        <f>INDEX(L:L, MATCH(A55, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>1.08</v>
       </c>
       <c r="E55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K55" t="s">
@@ -4065,11 +3530,11 @@
         <v>5.620999813079834</v>
       </c>
       <c r="C56">
-        <f>INDEX(L:L, MATCH(A56, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="E56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="K56" t="s">
@@ -4087,11 +3552,11 @@
         <v>5.6110000610351562</v>
       </c>
       <c r="C57">
-        <f>INDEX(L:L, MATCH(A57, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K57" t="s">
@@ -4109,11 +3574,11 @@
         <v>5.5689997673034668</v>
       </c>
       <c r="C58">
-        <f>INDEX(L:L, MATCH(A58, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>1.07</v>
       </c>
       <c r="E58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="K58" t="s">
@@ -4134,11 +3599,11 @@
         <v>5.5250000953674316</v>
       </c>
       <c r="C59">
-        <f>INDEX(L:L, MATCH(A59, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K59" t="s">
@@ -4156,11 +3621,11 @@
         <v>5.5</v>
       </c>
       <c r="C60">
-        <f>INDEX(L:L, MATCH(A60, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="E60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="K60" t="s">
@@ -4178,11 +3643,11 @@
         <v>5.4930000305175781</v>
       </c>
       <c r="C61">
-        <f>INDEX(L:L, MATCH(A61, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
       <c r="E61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="K61" t="s">
@@ -4200,11 +3665,11 @@
         <v>5.429999828338623</v>
       </c>
       <c r="C62">
-        <f>INDEX(L:L, MATCH(A62, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>0.74</v>
       </c>
       <c r="E62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K62" t="s">
@@ -4225,11 +3690,11 @@
         <v>5.3949999809265137</v>
       </c>
       <c r="C63">
-        <f>INDEX(L:L, MATCH(A63, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
       <c r="E63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="K63" t="s">
@@ -4250,11 +3715,11 @@
         <v>5.3359999656677246</v>
       </c>
       <c r="C64">
-        <f>INDEX(L:L, MATCH(A64, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="K64" t="s">
@@ -4275,11 +3740,11 @@
         <v>5.3239998817443848</v>
       </c>
       <c r="C65">
-        <f>INDEX(L:L, MATCH(A65, K:K, 0))</f>
+        <f t="shared" si="2"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="E65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
       <c r="K65" t="s">
@@ -4300,11 +3765,11 @@
         <v>5.310999870300293</v>
       </c>
       <c r="C66">
-        <f>INDEX(L:L, MATCH(A66, K:K, 0))</f>
+        <f t="shared" ref="C66:C97" si="3">INDEX(L:L, MATCH(A66, K:K, 0))</f>
         <v>7.21</v>
       </c>
       <c r="E66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K66" t="s">
@@ -4325,11 +3790,11 @@
         <v>5.2930002212524414</v>
       </c>
       <c r="C67">
-        <f>INDEX(L:L, MATCH(A67, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E130" si="1">INDEX(O:O, MATCH(A67, K:K, 0))</f>
+        <f t="shared" ref="E67:E130" si="4">INDEX(O:O, MATCH(A67, K:K, 0))</f>
         <v>1.2</v>
       </c>
       <c r="K67" t="s">
@@ -4347,11 +3812,11 @@
         <v>5.2729997634887695</v>
       </c>
       <c r="C68">
-        <f>INDEX(L:L, MATCH(A68, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K68" t="s">
@@ -4372,11 +3837,11 @@
         <v>5.2690000534057617</v>
       </c>
       <c r="C69">
-        <f>INDEX(L:L, MATCH(A69, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>3.6</v>
       </c>
       <c r="E69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.23</v>
       </c>
       <c r="K69" t="s">
@@ -4397,11 +3862,11 @@
         <v>5.2620000839233398</v>
       </c>
       <c r="C70">
-        <f>INDEX(L:L, MATCH(A70, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="E70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K70" t="s">
@@ -4422,11 +3887,11 @@
         <v>5.2369999885559082</v>
       </c>
       <c r="C71">
-        <f>INDEX(L:L, MATCH(A71, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>1.9</v>
       </c>
       <c r="E71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="K71" t="s">
@@ -4447,11 +3912,11 @@
         <v>5.2350001335144043</v>
       </c>
       <c r="C72">
-        <f>INDEX(L:L, MATCH(A72, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>4.22</v>
       </c>
       <c r="E72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K72" t="s">
@@ -4472,11 +3937,11 @@
         <v>5.2340002059936523</v>
       </c>
       <c r="C73">
-        <f>INDEX(L:L, MATCH(A73, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
       <c r="E73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K73" t="s">
@@ -4494,11 +3959,11 @@
         <v>5.2300000190734863</v>
       </c>
       <c r="C74">
-        <f>INDEX(L:L, MATCH(A74, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0.31</v>
       </c>
       <c r="E74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.98</v>
       </c>
       <c r="K74" t="s">
@@ -4516,11 +3981,11 @@
         <v>5.2270002365112305</v>
       </c>
       <c r="C75">
-        <f>INDEX(L:L, MATCH(A75, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>1.7</v>
       </c>
       <c r="E75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.78</v>
       </c>
       <c r="K75" t="s">
@@ -4541,11 +4006,11 @@
         <v>5.2249999046325684</v>
       </c>
       <c r="C76">
-        <f>INDEX(L:L, MATCH(A76, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K76" t="s">
@@ -4566,11 +4031,11 @@
         <v>5.195000171661377</v>
       </c>
       <c r="C77">
-        <f>INDEX(L:L, MATCH(A77, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>2.7</v>
       </c>
       <c r="E77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.4</v>
       </c>
       <c r="K77" t="s">
@@ -4594,11 +4059,11 @@
         <v>5.1820001602172852</v>
       </c>
       <c r="C78">
-        <f>INDEX(L:L, MATCH(A78, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
       <c r="E78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="K78" t="s">
@@ -4619,11 +4084,11 @@
         <v>5.1810002326965332</v>
       </c>
       <c r="C79">
-        <f>INDEX(L:L, MATCH(A79, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0.83</v>
       </c>
       <c r="E79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="K79" t="s">
@@ -4641,11 +4106,11 @@
         <v>5.1510000228881836</v>
       </c>
       <c r="C80">
-        <f>INDEX(L:L, MATCH(A80, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K80" t="s">
@@ -4666,11 +4131,11 @@
         <v>5.0739998817443848</v>
       </c>
       <c r="C81">
-        <f>INDEX(L:L, MATCH(A81, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>14.3</v>
       </c>
       <c r="E81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K81" t="s">
@@ -4694,11 +4159,11 @@
         <v>5.0409998893737793</v>
       </c>
       <c r="C82">
-        <f>INDEX(L:L, MATCH(A82, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
       <c r="K82" t="s">
@@ -4719,11 +4184,11 @@
         <v>5.0110001564025879</v>
       </c>
       <c r="C83">
-        <f>INDEX(L:L, MATCH(A83, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>4.2</v>
       </c>
       <c r="E83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.88</v>
       </c>
       <c r="K83" t="s">
@@ -4747,11 +4212,11 @@
         <v>5.004000186920166</v>
       </c>
       <c r="C84">
-        <f>INDEX(L:L, MATCH(A84, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
       <c r="K84" t="s">
@@ -4772,11 +4237,11 @@
         <v>4.9619998931884766</v>
       </c>
       <c r="C85">
-        <f>INDEX(L:L, MATCH(A85, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
       <c r="K85" t="s">
@@ -4794,11 +4259,11 @@
         <v>4.9549999237060547</v>
       </c>
       <c r="C86">
-        <f>INDEX(L:L, MATCH(A86, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K86" t="s">
@@ -4822,11 +4287,11 @@
         <v>4.8289999961853027</v>
       </c>
       <c r="C87">
-        <f>INDEX(L:L, MATCH(A87, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>3.65</v>
       </c>
       <c r="E87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K87" t="s">
@@ -4844,11 +4309,11 @@
         <v>4.804999828338623</v>
       </c>
       <c r="C88">
-        <f>INDEX(L:L, MATCH(A88, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>2.5961382443615131</v>
       </c>
       <c r="E88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K88" t="s">
@@ -4869,11 +4334,11 @@
         <v>4.7350001335144043</v>
       </c>
       <c r="C89">
-        <f>INDEX(L:L, MATCH(A89, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>6.24</v>
       </c>
       <c r="E89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.05</v>
       </c>
       <c r="K89" t="s">
@@ -4897,11 +4362,11 @@
         <v>4.7140002250671387</v>
       </c>
       <c r="C90">
-        <f>INDEX(L:L, MATCH(A90, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
       <c r="E90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K90" t="s">
@@ -4922,11 +4387,11 @@
         <v>4.7090001106262207</v>
       </c>
       <c r="C91">
-        <f>INDEX(L:L, MATCH(A91, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>5.42</v>
       </c>
       <c r="E91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K91" t="s">
@@ -4950,11 +4415,11 @@
         <v>4.695000171661377</v>
       </c>
       <c r="C92">
-        <f>INDEX(L:L, MATCH(A92, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K92" t="s">
@@ -4978,11 +4443,11 @@
         <v>4.6440000534057617</v>
       </c>
       <c r="C93">
-        <f>INDEX(L:L, MATCH(A93, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>1.8</v>
       </c>
       <c r="E93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="K93" t="s">
@@ -5003,11 +4468,11 @@
         <v>4.6079998016357422</v>
       </c>
       <c r="C94">
-        <f>INDEX(L:L, MATCH(A94, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>3.3</v>
       </c>
       <c r="E94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="K94" t="s">
@@ -5028,11 +4493,11 @@
         <v>4.5739998817443848</v>
       </c>
       <c r="C95">
-        <f>INDEX(L:L, MATCH(A95, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.02</v>
       </c>
       <c r="K95" t="s">
@@ -5056,11 +4521,11 @@
         <v>4.5529999732971191</v>
       </c>
       <c r="C96">
-        <f>INDEX(L:L, MATCH(A96, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>2.1</v>
       </c>
       <c r="E96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
       <c r="K96" t="s">
@@ -5084,11 +4549,11 @@
         <v>4.5500001907348633</v>
       </c>
       <c r="C97">
-        <f>INDEX(L:L, MATCH(A97, K:K, 0))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K97" t="s">
@@ -5112,11 +4577,11 @@
         <v>4.5450000762939453</v>
       </c>
       <c r="C98">
-        <f>INDEX(L:L, MATCH(A98, K:K, 0))</f>
+        <f t="shared" ref="C98:C134" si="5">INDEX(L:L, MATCH(A98, K:K, 0))</f>
         <v>0.94</v>
       </c>
       <c r="E98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.07</v>
       </c>
       <c r="K98" t="s">
@@ -5140,11 +4605,11 @@
         <v>4.5349998474121094</v>
       </c>
       <c r="C99">
-        <f>INDEX(L:L, MATCH(A99, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K99" t="s">
@@ -5168,11 +4633,11 @@
         <v>4.5139999389648438</v>
       </c>
       <c r="C100">
-        <f>INDEX(L:L, MATCH(A100, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>9.5</v>
       </c>
       <c r="E100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K100" t="s">
@@ -5196,11 +4661,11 @@
         <v>4.4970002174377441</v>
       </c>
       <c r="C101">
-        <f>INDEX(L:L, MATCH(A101, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K101" t="s">
@@ -5224,11 +4689,11 @@
         <v>4.4650001525878906</v>
       </c>
       <c r="C102">
-        <f>INDEX(L:L, MATCH(A102, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K102" t="s">
@@ -5249,11 +4714,11 @@
         <v>4.4600000381469727</v>
       </c>
       <c r="C103">
-        <f>INDEX(L:L, MATCH(A103, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K103" t="s">
@@ -5277,11 +4742,11 @@
         <v>4.440000057220459</v>
       </c>
       <c r="C104">
-        <f>INDEX(L:L, MATCH(A104, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>1.43</v>
       </c>
       <c r="E104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="K104" t="s">
@@ -5305,11 +4770,11 @@
         <v>4.375999927520752</v>
       </c>
       <c r="C105">
-        <f>INDEX(L:L, MATCH(A105, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>3.5</v>
       </c>
       <c r="E105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K105" t="s">
@@ -5333,11 +4798,11 @@
         <v>4.315000057220459</v>
       </c>
       <c r="C106">
-        <f>INDEX(L:L, MATCH(A106, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.52</v>
       </c>
       <c r="K106" t="s">
@@ -5361,11 +4826,11 @@
         <v>4.2919998168945312</v>
       </c>
       <c r="C107">
-        <f>INDEX(L:L, MATCH(A107, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K107" t="s">
@@ -5389,11 +4854,11 @@
         <v>4.2859997749328613</v>
       </c>
       <c r="C108">
-        <f>INDEX(L:L, MATCH(A108, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>2.7</v>
       </c>
       <c r="E108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
       <c r="K108" t="s">
@@ -5417,11 +4882,11 @@
         <v>4.190000057220459</v>
       </c>
       <c r="C109">
-        <f>INDEX(L:L, MATCH(A109, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="K109" t="s">
@@ -5442,11 +4907,11 @@
         <v>4.1680002212524414</v>
       </c>
       <c r="C110">
-        <f>INDEX(L:L, MATCH(A110, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>3.5</v>
       </c>
       <c r="E110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K110" t="s">
@@ -5467,11 +4932,11 @@
         <v>4.1389999389648438</v>
       </c>
       <c r="C111">
-        <f>INDEX(L:L, MATCH(A111, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K111" t="s">
@@ -5495,11 +4960,11 @@
         <v>4.119999885559082</v>
       </c>
       <c r="C112">
-        <f>INDEX(L:L, MATCH(A112, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K112" t="s">
@@ -5523,11 +4988,11 @@
         <v>4.0960001945495605</v>
       </c>
       <c r="C113">
-        <f>INDEX(L:L, MATCH(A113, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>2.9</v>
       </c>
       <c r="E113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K113" t="s">
@@ -5551,11 +5016,11 @@
         <v>4.0809998512268066</v>
       </c>
       <c r="C114">
-        <f>INDEX(L:L, MATCH(A114, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
       <c r="K114" t="s">
@@ -5579,11 +5044,11 @@
         <v>4.0320000648498535</v>
       </c>
       <c r="C115">
-        <f>INDEX(L:L, MATCH(A115, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>2.9</v>
       </c>
       <c r="E115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K115" t="s">
@@ -5607,11 +5072,11 @@
         <v>4.0279998779296875</v>
       </c>
       <c r="C116">
-        <f>INDEX(L:L, MATCH(A116, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K116" t="s">
@@ -5635,11 +5100,11 @@
         <v>3.9700000286102295</v>
       </c>
       <c r="C117">
-        <f>INDEX(L:L, MATCH(A117, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K117" t="s">
@@ -5657,11 +5122,11 @@
         <v>3.9360001087188721</v>
       </c>
       <c r="C118">
-        <f>INDEX(L:L, MATCH(A118, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K118" t="s">
@@ -5682,11 +5147,11 @@
         <v>3.875</v>
       </c>
       <c r="C119">
-        <f>INDEX(L:L, MATCH(A119, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
       <c r="K119" t="s">
@@ -5707,11 +5172,11 @@
         <v>3.8080000877380371</v>
       </c>
       <c r="C120">
-        <f>INDEX(L:L, MATCH(A120, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K120" t="s">
@@ -5735,11 +5200,11 @@
         <v>3.7950000762939453</v>
       </c>
       <c r="C121">
-        <f>INDEX(L:L, MATCH(A121, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K121" t="s">
@@ -5763,11 +5228,11 @@
         <v>3.7939999103546143</v>
       </c>
       <c r="C122">
-        <f>INDEX(L:L, MATCH(A122, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>4.28</v>
       </c>
       <c r="E122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K122" t="s">
@@ -5791,11 +5256,11 @@
         <v>3.7660000324249268</v>
       </c>
       <c r="C123">
-        <f>INDEX(L:L, MATCH(A123, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K123" t="s">
@@ -5819,11 +5284,11 @@
         <v>3.6570000648498535</v>
       </c>
       <c r="C124">
-        <f>INDEX(L:L, MATCH(A124, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.23</v>
       </c>
       <c r="K124" t="s">
@@ -5847,11 +5312,11 @@
         <v>3.6440000534057617</v>
       </c>
       <c r="C125">
-        <f>INDEX(L:L, MATCH(A125, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>9.1</v>
       </c>
       <c r="E125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K125" t="s">
@@ -5872,11 +5337,11 @@
         <v>3.6029999256134033</v>
       </c>
       <c r="C126">
-        <f>INDEX(L:L, MATCH(A126, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>1.51</v>
       </c>
       <c r="E126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K126" t="s">
@@ -5897,11 +5362,11 @@
         <v>3.5929999351501465</v>
       </c>
       <c r="C127">
-        <f>INDEX(L:L, MATCH(A127, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="K127" t="s">
@@ -5925,11 +5390,11 @@
         <v>3.5910000801086426</v>
       </c>
       <c r="C128">
-        <f>INDEX(L:L, MATCH(A128, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K128" t="s">
@@ -5953,11 +5418,11 @@
         <v>3.5329999923706055</v>
       </c>
       <c r="C129">
-        <f>INDEX(L:L, MATCH(A129, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>3.18</v>
       </c>
       <c r="E129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K129" t="s">
@@ -5981,11 +5446,11 @@
         <v>3.5069999694824219</v>
       </c>
       <c r="C130">
-        <f>INDEX(L:L, MATCH(A130, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K130" t="s">
@@ -6006,11 +5471,11 @@
         <v>3.494999885559082</v>
       </c>
       <c r="C131">
-        <f>INDEX(L:L, MATCH(A131, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E131">
-        <f t="shared" ref="E131:E134" si="2">INDEX(O:O, MATCH(A131, K:K, 0))</f>
+        <f t="shared" ref="E131:E134" si="6">INDEX(O:O, MATCH(A131, K:K, 0))</f>
         <v>0</v>
       </c>
       <c r="K131" t="s">
@@ -6031,11 +5496,11 @@
         <v>3.4709999561309814</v>
       </c>
       <c r="C132">
-        <f>INDEX(L:L, MATCH(A132, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K132" t="s">
@@ -6056,11 +5521,11 @@
         <v>2.9049999713897705</v>
       </c>
       <c r="C133">
-        <f>INDEX(L:L, MATCH(A133, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K133" t="s">
@@ -6081,11 +5546,11 @@
         <v>2.6930000782012939</v>
       </c>
       <c r="C134">
-        <f>INDEX(L:L, MATCH(A134, K:K, 0))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K134" t="s">

</xml_diff>

<commit_message>
added more oecd countries and missing data
</commit_message>
<xml_diff>
--- a/Stephanie/happiness-correlations-steph.xlsx
+++ b/Stephanie/happiness-correlations-steph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="460" windowWidth="22160" windowHeight="16540" activeTab="2" xr2:uid="{05585DEE-E31A-F647-82F2-51A3607B14A8}"/>
+    <workbookView xWindow="1540" yWindow="2460" windowWidth="23040" windowHeight="16540" activeTab="2" xr2:uid="{05585DEE-E31A-F647-82F2-51A3607B14A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Happiness + Education Level" sheetId="1" r:id="rId1"/>
@@ -1166,7 +1166,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1722,7 +1722,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2210,7 +2210,7 @@
   <dimension ref="A1:Q299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>